<commit_message>
Adding the last page
</commit_message>
<xml_diff>
--- a/public/meyvali-excel.xlsx
+++ b/public/meyvali-excel.xlsx
@@ -5,18 +5,19 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\-Downloads-\Study\BM\Staj\2 MaPos\Meyvalı Lokantası\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\-Downloads-\Study\BM\Staj\2 MaPos\Meyvalı Lokantası\meyvali-excel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC19553-D34A-464C-9789-8039F2816CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C409B27-5635-41F9-A4AD-20F49A4AE391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -974,7 +975,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -5817,4 +5818,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211B0F78-C49C-457D-9954-525E437F6D61}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sheets Indexes Fix and Renaming
</commit_message>
<xml_diff>
--- a/public/meyvali-excel.xlsx
+++ b/public/meyvali-excel.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\-Downloads-\Study\BM\Staj\2 MaPos\Meyvalı Lokantası\meyvali-excel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C423D7B4-21BF-4949-86F6-229F17586395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4EFA5C-CC21-4001-A9D6-F906E87C6E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Urunler" sheetId="3" r:id="rId2"/>
+    <sheet name="Odeme ve Tahsilat" sheetId="4" r:id="rId3"/>
+    <sheet name="Gun Sonu" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>SUT</t>
   </si>
@@ -171,151 +170,13 @@
     <t>K</t>
   </si>
   <si>
-    <t>hal - Pazar</t>
-  </si>
-  <si>
-    <t>tutar</t>
-  </si>
-  <si>
-    <t>ekmek</t>
-  </si>
-  <si>
-    <t>nakit</t>
-  </si>
-  <si>
-    <t>süt</t>
-  </si>
-  <si>
-    <t>kasadan</t>
-  </si>
-  <si>
-    <t>özkardeşler</t>
-  </si>
-  <si>
-    <t>kredi kartı</t>
-  </si>
-  <si>
-    <t>adisyon no</t>
-  </si>
-  <si>
-    <t>ödeme cinsi</t>
-  </si>
-  <si>
-    <t>havale</t>
-  </si>
-  <si>
-    <t>resim</t>
-  </si>
-  <si>
-    <t>onay</t>
-  </si>
-  <si>
-    <t>kasa raporu</t>
-  </si>
-  <si>
-    <t>açıklama</t>
-  </si>
-  <si>
-    <t>b.para</t>
-  </si>
-  <si>
-    <t>kasa</t>
-  </si>
-  <si>
-    <t>tahislat eski bakiye kredi kartı</t>
-  </si>
-  <si>
-    <t>tahsilat eski bakiye nakit</t>
-  </si>
-  <si>
-    <t>tahsilat eski bakiye havale</t>
-  </si>
-  <si>
-    <t>toplam nakit</t>
-  </si>
-  <si>
-    <t>gün başı</t>
-  </si>
-  <si>
-    <t>saat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">su </t>
-  </si>
-  <si>
-    <t>havele</t>
-  </si>
-  <si>
-    <t>ÜRÜN</t>
-  </si>
-  <si>
-    <t>ADET / KG</t>
-  </si>
-  <si>
-    <t>TUTAR</t>
-  </si>
-  <si>
-    <t>ÖDEME TÜRÜ</t>
-  </si>
-  <si>
-    <t>KATEGORİ</t>
-  </si>
-  <si>
-    <t>DEĞİŞİKLİK YAP</t>
-  </si>
-  <si>
-    <t>BELGE /RESİM</t>
-  </si>
-  <si>
-    <t>ONAYLA VE KAYDET</t>
-  </si>
-  <si>
-    <t>NOTLAR</t>
-  </si>
-  <si>
-    <t>Aynı gün içerisinde aynı kategoride farklı ürünler alınmış olabilir. Bunların bizim özet tablomuzda kategori kısmında toplamı gözükmesi gerekir.</t>
-  </si>
-  <si>
-    <t>İstediğimiz zaman kategori açabiliyor olmamız gerekiyor.</t>
-  </si>
-  <si>
-    <t>Sambaposla entegrasyon; ana ekrandaki sambapos hücresine toplam ciro, paket adet ve toplam paket tutar kısımları gelmesi gerekiyor. Veresiye ve ikram satırları " adisyon ödeme yöntemi " yle senkron olamsı gerekiyor.</t>
-  </si>
-  <si>
-    <t>günsonu - gönder kısmı; normal onay kısımları onaylanmadan gün sonu yapılamasın.</t>
-  </si>
-  <si>
     <t>not / olay günlük</t>
   </si>
   <si>
-    <t>not / olay günlük açıklama</t>
-  </si>
-  <si>
-    <t>Günsonu - Gönder</t>
-  </si>
-  <si>
     <t>gün başı saat</t>
   </si>
   <si>
     <t>gün sonu saat</t>
-  </si>
-  <si>
-    <t>adisyon ödeme ve tahsilat yöntemi</t>
-  </si>
-  <si>
-    <t>Adisyon ve tahsilat yönetimi ; tahsilatlar veresiye hanesinden ( veya tahsil edilmiş adisyondan düşülecek )</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>ÜRÜN ADI GİRİNİZ</t>
-  </si>
-  <si>
-    <t>ONAY</t>
-  </si>
-  <si>
-    <t>Değişiklikler; yapılan her değişiklik ana özet tablomuzda " hayalet şeklinde gözüksün " fakat hesaplarda etkili olmasın, ( yapılan değişiklikleri görmek hem kalifiye işçiliğe hemde olay duygu durmuna etki eder. ) ( ana ekranda " bir tuş " değişiklik yapıolanları gostermemesi için</t>
   </si>
   <si>
     <t>Pazar</t>
@@ -410,7 +271,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;TL&quot;;[Red]\-#,##0.00\ &quot;TL&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,22 +367,6 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -561,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -642,22 +487,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,18 +920,18 @@
         <v>24</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7">
         <v>5125</v>
@@ -1161,13 +990,13 @@
         <v>3075</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="AD2" s="36"/>
     </row>
     <row r="3" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="C3" s="7">
         <v>3750</v>
@@ -1223,7 +1052,7 @@
     </row>
     <row r="4" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="C4" s="7">
         <v>4500</v>
@@ -1281,7 +1110,7 @@
     </row>
     <row r="5" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C5" s="7">
         <v>3450</v>
@@ -1343,7 +1172,7 @@
     </row>
     <row r="6" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="C6" s="7">
         <v>4800</v>
@@ -1398,16 +1227,16 @@
         <v>3645</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="AC6" s="10" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="AD6" s="36"/>
     </row>
     <row r="7" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1465,7 +1294,7 @@
     </row>
     <row r="8" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1521,7 +1350,7 @@
     </row>
     <row r="9" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="C9" s="7">
         <v>4755</v>
@@ -1587,7 +1416,7 @@
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="C10" s="7">
         <v>3750</v>
@@ -1646,13 +1475,13 @@
         <v>2160</v>
       </c>
       <c r="AB10" s="10" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="AD10" s="36"/>
     </row>
     <row r="11" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="C11" s="7">
         <v>3875</v>
@@ -2562,7 +2391,7 @@
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="H34" s="7">
         <v>12000</v>
@@ -2571,14 +2400,14 @@
         <v>42935</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="7">
         <v>31993</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
@@ -2610,7 +2439,7 @@
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="H35" s="7">
         <v>22000</v>
@@ -2619,14 +2448,14 @@
         <v>76022</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="K35" s="7"/>
       <c r="L35" s="7">
         <v>19271</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
@@ -2654,7 +2483,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="H36" s="7">
         <v>136850</v>
@@ -2688,7 +2517,7 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="H37" s="7">
         <v>16064</v>
@@ -2722,7 +2551,7 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="H38" s="7">
         <v>10338</v>
@@ -2756,7 +2585,7 @@
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="H39" s="7">
         <v>15900</v>
@@ -2790,7 +2619,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="H40" s="7">
         <v>12377</v>
@@ -2824,7 +2653,7 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="H41" s="7">
         <v>4668</v>
@@ -2858,7 +2687,7 @@
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="H42" s="7">
         <v>4284</v>
@@ -2892,7 +2721,7 @@
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="H43" s="7">
         <v>7760</v>
@@ -2926,7 +2755,7 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="H44" s="7">
         <v>14450</v>
@@ -2960,7 +2789,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="H45" s="7">
         <v>96876</v>
@@ -2994,7 +2823,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="H46" s="7">
         <v>4070</v>
@@ -3028,7 +2857,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="H47" s="7">
         <v>5700</v>
@@ -3812,7 +3641,7 @@
         <v>20000</v>
       </c>
       <c r="F72" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="G72"/>
       <c r="H72"/>
@@ -5166,637 +4995,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="8" width="10" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="44">
-        <v>45286</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="40"/>
-    </row>
-    <row r="2" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="39">
-        <v>97</v>
-      </c>
-      <c r="C3" s="39">
-        <v>2865</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="K3" s="39">
-        <v>97</v>
-      </c>
-      <c r="L3" s="39">
-        <v>2865</v>
-      </c>
-      <c r="M3" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="40"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="40"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="40"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="39">
-        <v>200</v>
-      </c>
-      <c r="C7" s="39">
-        <v>1850</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="K7" s="39">
-        <v>200</v>
-      </c>
-      <c r="L7" s="39">
-        <v>1850</v>
-      </c>
-      <c r="M7" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O7" s="40"/>
-    </row>
-    <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39">
-        <v>5285</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39">
-        <v>5285</v>
-      </c>
-      <c r="M8" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="40"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="39">
-        <v>137</v>
-      </c>
-      <c r="C9" s="39">
-        <v>48415</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="K9" s="39">
-        <v>137</v>
-      </c>
-      <c r="L9" s="39">
-        <v>48415</v>
-      </c>
-      <c r="M9" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" s="40"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="40"/>
-    </row>
-    <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="O11" s="40"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="39">
-        <v>16</v>
-      </c>
-      <c r="C12" s="39">
-        <v>4516</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="K12" s="39">
-        <v>16</v>
-      </c>
-      <c r="L12" s="39">
-        <v>4516</v>
-      </c>
-      <c r="M12" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="O13" s="40"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="O14" s="40"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="O16" s="40"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>300</v>
-      </c>
-      <c r="B20">
-        <v>21256</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>700</v>
-      </c>
-      <c r="B21">
-        <v>321516</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>10000</v>
-      </c>
-      <c r="B22">
-        <v>54656</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3800</v>
-      </c>
-      <c r="B23">
-        <v>54566</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6500</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>10000</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>5000</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>6000</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>21000</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>123000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A34" s="43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B455A097-A885-48EB-826D-DBA72521E163}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5808,7 +5006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CE7871-B7C9-44DF-BE42-3F23FF9E318D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5820,7 +5018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C2A7A-55FB-4AA4-883D-78EFD80FDE4A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Reodering the sheets and index full fix
</commit_message>
<xml_diff>
--- a/public/meyvali-excel.xlsx
+++ b/public/meyvali-excel.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\-Downloads-\Study\BM\Staj\2 MaPos\Meyvalı Lokantası\meyvali-excel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4EFA5C-CC21-4001-A9D6-F906E87C6E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F1756-190A-4514-BAE6-FF25A28334E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
-    <sheet name="Urunler" sheetId="3" r:id="rId2"/>
-    <sheet name="Odeme ve Tahsilat" sheetId="4" r:id="rId3"/>
-    <sheet name="Gun Sonu" sheetId="5" r:id="rId4"/>
+    <sheet name="Urun" sheetId="2" r:id="rId2"/>
+    <sheet name="Odeme ve Tahsilat" sheetId="3" r:id="rId3"/>
+    <sheet name="Gun Sonu" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4995,6 +4995,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B455A097-A885-48EB-826D-DBA72521E163}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5006,20 +5022,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CE7871-B7C9-44DF-BE42-3F23FF9E318D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C2A7A-55FB-4AA4-883D-78EFD80FDE4A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>